<commit_message>
adequacao tabela de custos do toner por periodo de tempo
</commit_message>
<xml_diff>
--- a/x.xlsx
+++ b/x.xlsx
@@ -448,10 +448,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -461,10 +461,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
@@ -474,10 +474,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="C4" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -487,10 +487,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6">
@@ -500,10 +500,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C6" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7">
@@ -513,10 +513,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
@@ -526,10 +526,10 @@
         </is>
       </c>
       <c r="B8" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" t="n">
         <v>0</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -539,10 +539,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
@@ -555,7 +555,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">
@@ -565,10 +565,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>39</v>
+        <v>196</v>
       </c>
       <c r="C11" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -578,10 +578,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C12" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -591,10 +591,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C13" t="n">
-        <v>7</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14">
@@ -604,10 +604,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>117</v>
+        <v>476</v>
       </c>
       <c r="C14" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -617,10 +617,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C15" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pronto para gerar dados
</commit_message>
<xml_diff>
--- a/x.xlsx
+++ b/x.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,6 +440,36 @@
       <c r="C1" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -448,10 +478,40 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>73</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>15</v>
+      </c>
+      <c r="M2" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="3">
@@ -461,10 +521,40 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>18</v>
+      </c>
+      <c r="I3" t="n">
         <v>12</v>
+      </c>
+      <c r="J3" t="n">
+        <v>6</v>
+      </c>
+      <c r="K3" t="n">
+        <v>26</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="4">
@@ -474,10 +564,40 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>32</v>
+        <v>111</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>183</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -487,10 +607,40 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>20</v>
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>47</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>75</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>33</v>
+      </c>
+      <c r="M5" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="6">
@@ -500,10 +650,40 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>8</v>
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>16</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>20</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -513,10 +693,40 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C7" t="n">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>36</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>28</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="8">
@@ -526,10 +736,40 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>14</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="9">
@@ -542,7 +782,37 @@
         <v>2</v>
       </c>
       <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
         <v>4</v>
+      </c>
+      <c r="F9" t="n">
+        <v>14</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>23</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>20</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -552,10 +822,40 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="C10" t="n">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>15</v>
+      </c>
+      <c r="E10" t="n">
+        <v>25</v>
+      </c>
+      <c r="F10" t="n">
+        <v>63</v>
+      </c>
+      <c r="G10" t="n">
+        <v>57</v>
+      </c>
+      <c r="H10" t="n">
+        <v>45</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>95</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="11">
@@ -565,9 +865,39 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>196</v>
+        <v>48</v>
       </c>
       <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>120</v>
+      </c>
+      <c r="E11" t="n">
+        <v>660</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>120</v>
+      </c>
+      <c r="H11" t="n">
+        <v>120</v>
+      </c>
+      <c r="I11" t="n">
+        <v>270</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>570</v>
+      </c>
+      <c r="M11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -578,10 +908,40 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>12</v>
+      </c>
+      <c r="F12" t="n">
+        <v>174</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>12</v>
+      </c>
+      <c r="K12" t="n">
+        <v>72</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="13">
@@ -591,10 +951,40 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>41</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>45</v>
+      </c>
+      <c r="I13" t="n">
+        <v>100</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>35</v>
+      </c>
+      <c r="L13" t="n">
+        <v>35</v>
+      </c>
+      <c r="M13" t="n">
+        <v>55</v>
       </c>
     </row>
     <row r="14">
@@ -604,10 +994,40 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>476</v>
+        <v>1715</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>981</v>
+      </c>
+      <c r="F14" t="n">
+        <v>880</v>
+      </c>
+      <c r="G14" t="n">
+        <v>770</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1760</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>440</v>
+      </c>
+      <c r="K14" t="n">
+        <v>330</v>
+      </c>
+      <c r="L14" t="n">
+        <v>770</v>
+      </c>
+      <c r="M14" t="n">
+        <v>550</v>
       </c>
     </row>
     <row r="15">
@@ -617,9 +1037,39 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>5</v>
+      </c>
+      <c r="E15" t="n">
+        <v>30</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>25</v>
+      </c>
+      <c r="H15" t="n">
+        <v>85</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>20</v>
+      </c>
+      <c r="K15" t="n">
+        <v>15</v>
+      </c>
+      <c r="L15" t="n">
+        <v>45</v>
+      </c>
+      <c r="M15" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modificacao - modelo considerando somente custo de compra
</commit_message>
<xml_diff>
--- a/x.xlsx
+++ b/x.xlsx
@@ -471,36 +471,16 @@
           <t>tn1</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>2</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0</v>
-      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -508,36 +488,16 @@
           <t>tn2</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>3</v>
-      </c>
-      <c r="C3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" t="n">
-        <v>3</v>
-      </c>
-      <c r="I3" t="n">
-        <v>3</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0</v>
-      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -545,36 +505,16 @@
           <t>tn3</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>2</v>
-      </c>
-      <c r="J4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -582,36 +522,16 @@
           <t>tn4</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0</v>
-      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -619,36 +539,16 @@
           <t>tn5</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" t="n">
-        <v>1</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" t="n">
-        <v>1</v>
-      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -656,36 +556,16 @@
           <t>tn6</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" t="n">
-        <v>2</v>
-      </c>
-      <c r="F7" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" t="n">
-        <v>1</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" t="n">
-        <v>1</v>
-      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -693,36 +573,16 @@
           <t>tn7</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" t="n">
-        <v>1</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" t="n">
-        <v>1</v>
-      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -730,36 +590,16 @@
           <t>tn8</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0</v>
-      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -767,36 +607,16 @@
           <t>tn9</t>
         </is>
       </c>
-      <c r="B10" t="n">
-        <v>2</v>
-      </c>
-      <c r="C10" t="n">
-        <v>4</v>
-      </c>
-      <c r="D10" t="n">
-        <v>85</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0</v>
-      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -804,36 +624,16 @@
           <t>tn10</t>
         </is>
       </c>
-      <c r="B11" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" t="n">
-        <v>9</v>
-      </c>
-      <c r="D11" t="n">
-        <v>71</v>
-      </c>
-      <c r="E11" t="n">
-        <v>57</v>
-      </c>
-      <c r="F11" t="n">
-        <v>72</v>
-      </c>
-      <c r="G11" t="n">
-        <v>16</v>
-      </c>
-      <c r="H11" t="n">
-        <v>30</v>
-      </c>
-      <c r="I11" t="n">
-        <v>153</v>
-      </c>
-      <c r="J11" t="n">
-        <v>40</v>
-      </c>
-      <c r="K11" t="n">
-        <v>7</v>
-      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -841,36 +641,16 @@
           <t>tn11</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v>38</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0</v>
-      </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -878,36 +658,16 @@
           <t>tn12</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" t="n">
-        <v>7</v>
-      </c>
-      <c r="D13" t="n">
-        <v>2</v>
-      </c>
-      <c r="E13" t="n">
-        <v>3</v>
-      </c>
-      <c r="F13" t="n">
-        <v>50</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" t="n">
-        <v>0</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0</v>
-      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -915,36 +675,16 @@
           <t>tn13</t>
         </is>
       </c>
-      <c r="B14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" t="n">
-        <v>63</v>
-      </c>
-      <c r="D14" t="n">
-        <v>136</v>
-      </c>
-      <c r="E14" t="n">
-        <v>108</v>
-      </c>
-      <c r="F14" t="n">
-        <v>146</v>
-      </c>
-      <c r="G14" t="n">
-        <v>91</v>
-      </c>
-      <c r="H14" t="n">
-        <v>114</v>
-      </c>
-      <c r="I14" t="n">
-        <v>106</v>
-      </c>
-      <c r="J14" t="n">
-        <v>65</v>
-      </c>
-      <c r="K14" t="n">
-        <v>29</v>
-      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -952,36 +692,16 @@
           <t>tn14</t>
         </is>
       </c>
-      <c r="B15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" t="n">
-        <v>31</v>
-      </c>
-      <c r="G15" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" t="n">
-        <v>0</v>
-      </c>
-      <c r="K15" t="n">
-        <v>1</v>
-      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>